<commit_message>
Fixed merge value in SpacesCSV file
</commit_message>
<xml_diff>
--- a/resource/SpacesWColours.xlsx
+++ b/resource/SpacesWColours.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\temp2015\OneDrive - University College Dublin\College\Year 5\SoftwareEng\Project\Code\gameoflife\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_30f9\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="95" documentId="8_{2915447A-8400-421F-ACB9-F6B02B55775C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{302A09BF-EEE7-4609-ADCF-301FBCC487FB}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{2915447A-8400-421F-ACB9-F6B02B55775C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{5A3B994F-C63B-4DDE-BDAC-652FEF35494E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7590" xr2:uid="{76940089-184E-4799-9FE6-578B5E059973}"/>
   </bookViews>
@@ -372,9 +372,6 @@
     <t>105_4_0</t>
   </si>
   <si>
-    <t>107_4_4</t>
-  </si>
-  <si>
     <t>111_4_0</t>
   </si>
   <si>
@@ -412,6 +409,9 @@
   </si>
   <si>
     <t>126_14_53</t>
+  </si>
+  <si>
+    <t>107_4_5</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1017,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>17</v>
@@ -1076,7 +1076,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G5" t="s">
         <v>0</v>
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>0</v>
@@ -1256,7 +1256,7 @@
         <v>0</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K8" t="s">
         <v>0</v>
@@ -1300,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>0</v>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K9" t="s">
         <v>0</v>
@@ -1368,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K10" t="s">
         <v>0</v>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>82</v>
@@ -1424,19 +1424,19 @@
         <v>0</v>
       </c>
       <c r="J11" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="K11" s="8" t="s">
+      <c r="L11" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="L11" s="5" t="s">
+      <c r="M11" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="N11" s="8" t="s">
         <v>124</v>
-      </c>
-      <c r="N11" s="8" t="s">
-        <v>125</v>
       </c>
       <c r="O11" t="s">
         <v>0</v>
@@ -2025,7 +2025,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="F22" t="s">
         <v>0</v>

</xml_diff>